<commit_message>
deal with the wait for the click action
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TC001_ShopClient_VerifyLogin.xlsx
+++ b/src/test/resources/testdata/TC001_ShopClient_VerifyLogin.xlsx
@@ -1,19 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ca-at-framework-template\selenium-template\src\test\resources\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8757A639-80F2-47FF-AFFF-F7393A792225}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Example Test" sheetId="1" r:id="rId4"/>
-    <sheet name="Format Abbr." sheetId="2" r:id="rId5"/>
-    <sheet name="Readme" sheetId="3" r:id="rId6"/>
+    <sheet name="Example Test" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Username</t>
   </si>
@@ -21,188 +28,33 @@
     <t>Password</t>
   </si>
   <si>
-    <t>githubfengyun</t>
+    <t>csadmin</t>
   </si>
   <si>
-    <t>github888888</t>
-  </si>
-  <si>
-    <t>http://www.cmu.edu/blackboard</t>
-  </si>
-  <si>
-    <t>Question Format Abbreviations</t>
-  </si>
-  <si>
-    <t>Abbreviation</t>
-  </si>
-  <si>
-    <t>Question Type</t>
-  </si>
-  <si>
-    <t>MC</t>
-  </si>
-  <si>
-    <t>Multiple Choice</t>
-  </si>
-  <si>
-    <t>MA</t>
-  </si>
-  <si>
-    <t>Multiple Answer</t>
-  </si>
-  <si>
-    <t>TF</t>
-  </si>
-  <si>
-    <t>True/False</t>
-  </si>
-  <si>
-    <t>ESS</t>
-  </si>
-  <si>
-    <t>Essay</t>
-  </si>
-  <si>
-    <t>ORD</t>
-  </si>
-  <si>
-    <t>Ordering</t>
-  </si>
-  <si>
-    <t>MAT</t>
-  </si>
-  <si>
-    <t>Matching</t>
-  </si>
-  <si>
-    <t>FIB</t>
-  </si>
-  <si>
-    <t>Fill in the Blank</t>
-  </si>
-  <si>
-    <t>FIL</t>
-  </si>
-  <si>
-    <t>File response</t>
-  </si>
-  <si>
-    <t>NUM</t>
-  </si>
-  <si>
-    <t>Numeric Response</t>
-  </si>
-  <si>
-    <t>SR</t>
-  </si>
-  <si>
-    <t>Short response</t>
-  </si>
-  <si>
-    <t>OP</t>
-  </si>
-  <si>
-    <t>Opinion</t>
-  </si>
-  <si>
-    <t>FIB_PLUS</t>
-  </si>
-  <si>
-    <t>Multiple Fill in the Blank</t>
-  </si>
-  <si>
-    <t>JUMBLED_SENTENCE</t>
-  </si>
-  <si>
-    <t>Jumbled Sentence</t>
-  </si>
-  <si>
-    <t>QUIZ_BOWL</t>
-  </si>
-  <si>
-    <t>Quiz Bowl</t>
-  </si>
-  <si>
-    <t>File Information</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>http://www.cmu.edu/blackboard/files/evaluate/tests-example.xls</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>1.0 (January 2012)</t>
-  </si>
-  <si>
-    <t>Contact</t>
-  </si>
-  <si>
-    <t>bb-help@andrew.cmu.edu</t>
-  </si>
-  <si>
-    <t>About</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>This is an example and template for preparing Blackboard tests offline. See the full directions at:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="11"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> http://www.cmu.edu/blackboard/evaluate#manage_tests/import_questions</t>
-    </r>
+    <t>123abc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="11"/>
-      <name val="Arial"/>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -244,186 +96,101 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff0000d4"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FF0000D4"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>77390</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>72320</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1371748</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>49918</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="image.png" descr="image.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1">
-          <a:extLst/>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="77390" y="72319"/>
-          <a:ext cx="3275559" cy="302720"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>75307</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>72320</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>692310</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>49918</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="image.png" descr="image.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId1">
-          <a:extLst/>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="75307" y="72319"/>
-          <a:ext cx="3245904" cy="302720"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -625,7 +392,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -644,7 +411,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -674,7 +441,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -700,7 +467,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -726,7 +493,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -752,7 +519,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -778,7 +545,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -804,7 +571,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -830,7 +597,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -856,7 +623,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -882,7 +649,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -895,9 +662,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -914,7 +687,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -933,7 +706,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -959,7 +732,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -985,7 +758,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1011,7 +784,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1037,7 +810,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1063,7 +836,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1089,7 +862,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1115,7 +888,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1141,7 +914,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1167,7 +940,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1180,9 +953,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1196,7 +975,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1215,7 +994,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1245,7 +1024,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1271,7 +1050,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1297,7 +1076,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1323,7 +1102,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1349,7 +1128,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1375,7 +1154,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1401,7 +1180,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1427,7 +1206,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1453,7 +1232,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1466,41 +1245,48 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:IV2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8333" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.8516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" style="1" customWidth="1"/>
-    <col min="10" max="256" width="11.8516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="1" customWidth="1"/>
+    <col min="7" max="9" width="11.42578125" style="1" customWidth="1"/>
+    <col min="10" max="256" width="11.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3"/>
@@ -1511,11 +1297,11 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="2">
+    <row r="2" spans="1:9" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="3"/>
@@ -1527,475 +1313,12 @@
       <c r="I2" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05278" bottom="1.05278" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;K000000Example Test</oddHeader>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8333" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="1" width="26" style="4" customWidth="1"/>
-    <col min="2" max="2" width="26" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="4" customWidth="1"/>
-    <col min="6" max="256" width="11.8516" style="4" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="12.8" customHeight="1">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" ht="12.8" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" ht="12.8" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" ht="12.8" customHeight="1">
-      <c r="A4" t="s" s="6">
-        <v>4</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" ht="12.8" customHeight="1">
-      <c r="A5" s="5"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" ht="12.8" customHeight="1">
-      <c r="A6" t="s" s="8">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" ht="12.8" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" ht="12.8" customHeight="1">
-      <c r="A8" t="s" s="9">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s" s="9">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" ht="12.8" customHeight="1">
-      <c r="A9" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" ht="12.8" customHeight="1">
-      <c r="A10" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" ht="12.8" customHeight="1">
-      <c r="A11" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" ht="12.8" customHeight="1">
-      <c r="A12" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" ht="12.8" customHeight="1">
-      <c r="A13" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" ht="12.8" customHeight="1">
-      <c r="A14" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" ht="12.8" customHeight="1">
-      <c r="A15" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="B15" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" ht="12.8" customHeight="1">
-      <c r="A16" t="s" s="2">
-        <v>22</v>
-      </c>
-      <c r="B16" t="s" s="2">
-        <v>23</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" ht="12.8" customHeight="1">
-      <c r="A17" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="B17" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" ht="12.8" customHeight="1">
-      <c r="A18" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="B18" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" ht="12.8" customHeight="1">
-      <c r="A19" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="B19" t="s" s="2">
-        <v>29</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" ht="12.8" customHeight="1">
-      <c r="A20" t="s" s="2">
-        <v>30</v>
-      </c>
-      <c r="B20" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" ht="12.8" customHeight="1">
-      <c r="A21" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="B21" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" ht="12.8" customHeight="1">
-      <c r="A22" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="B22" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B7"/>
-    <mergeCell ref="A1:B3"/>
-  </mergeCells>
-  <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;K000000Format Abbr.</oddHeader>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8333" defaultRowHeight="12.8" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="1" width="11.5" style="10" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="10" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="10" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="10" customWidth="1"/>
-    <col min="5" max="5" width="19.3516" style="10" customWidth="1"/>
-    <col min="6" max="256" width="11.8516" style="10" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="12.8" customHeight="1">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" ht="12.8" customHeight="1">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" ht="12.8" customHeight="1">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" ht="12.8" customHeight="1">
-      <c r="A4" t="s" s="11">
-        <v>4</v>
-      </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" ht="12.8" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" ht="12.8" customHeight="1">
-      <c r="A6" t="s" s="8">
-        <v>36</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" ht="12.8" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" ht="12.8" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" ht="12.8" customHeight="1">
-      <c r="A9" t="s" s="13">
-        <v>37</v>
-      </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-    </row>
-    <row r="10" ht="12.8" customHeight="1">
-      <c r="A10" t="s" s="6">
-        <v>38</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" ht="12.8" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" ht="12.8" customHeight="1">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" ht="12.8" customHeight="1">
-      <c r="A13" t="s" s="13">
-        <v>39</v>
-      </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-    </row>
-    <row r="14" ht="12.8" customHeight="1">
-      <c r="A14" t="s" s="6">
-        <v>40</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" ht="12.8" customHeight="1">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" ht="12.8" customHeight="1">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" ht="12.8" customHeight="1">
-      <c r="A17" t="s" s="13">
-        <v>41</v>
-      </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-    </row>
-    <row r="18" ht="12.8" customHeight="1">
-      <c r="A18" t="s" s="6">
-        <v>42</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" ht="12.8" customHeight="1">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" ht="12.8" customHeight="1">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" ht="12.8" customHeight="1">
-      <c r="A21" t="s" s="13">
-        <v>43</v>
-      </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-    </row>
-    <row r="22" ht="35.05" customHeight="1">
-      <c r="A22" t="s" s="15">
-        <v>44</v>
-      </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-    </row>
-  </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A18:E19"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E15"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A10:E11"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A6:E7"/>
-    <mergeCell ref="A1:E3"/>
-  </mergeCells>
-  <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;K000000Readme</oddHeader>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>